<commit_message>
Added Rewrite Transaction In Selenium to Excel class
</commit_message>
<xml_diff>
--- a/premium calculations.xlsx
+++ b/premium calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WorkSpace\PolicyCenter_TESTING\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E941E7-92F5-49FF-B18B-1CDBAD365545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF441CB3-0A12-4DAA-8847-3B270E3C4148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="15">
   <si>
     <t>Label</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>issuance</t>
+  </si>
+  <si>
+    <t>Issuance</t>
+  </si>
+  <si>
+    <t>Change</t>
   </si>
 </sst>
 </file>
@@ -423,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,7 +441,7 @@
     <col min="4" max="4" customWidth="true" width="16.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -443,7 +449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -451,10 +457,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D7" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>13</v>
+      </c>
+      <c r="M10" t="s">
+        <v>10</v>
+      </c>
+      <c r="N10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -463,8 +480,23 @@
         <v>9</v>
       </c>
       <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="L12" t="s">
+        <v>14</v>
+      </c>
+      <c r="M12" t="s">
+        <v>10</v>
+      </c>
+      <c r="N12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -475,12 +507,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>

</xml_diff>